<commit_message>
clean up of unneeded files
</commit_message>
<xml_diff>
--- a/niceSchedule.xlsx
+++ b/niceSchedule.xlsx
@@ -473,27 +473,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>meili, troy</t>
+          <t>worker 13, worker 15</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>brandon, thomas, troy</t>
+          <t>worker 13, worker 15</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>meili, troy</t>
+          <t>worker 3, worker 13, worker 15</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>meili, troy</t>
+          <t>worker 13, worker 15</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>meili, troy</t>
+          <t>worker 13, worker 15</t>
         </is>
       </c>
     </row>
@@ -505,27 +505,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>chloe, makayla</t>
+          <t>worker 4, worker 9</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>andrew, thomas</t>
+          <t>worker 2, worker 6</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>chloe, makayla</t>
+          <t>worker 3, worker 9</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>andrew, jess</t>
+          <t>worker 2, worker 6</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>chloe, jess</t>
+          <t>worker 3, worker 6</t>
         </is>
       </c>
     </row>
@@ -537,27 +537,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>levi, meili</t>
+          <t>worker 8, worker 9</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>andrew, brandon</t>
+          <t>worker 2, worker 12</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>levi, makayla</t>
+          <t>worker 8, worker 9</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>andrew, jess</t>
+          <t>worker 2, worker 16</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>jess, levi</t>
+          <t>worker 6, worker 9</t>
         </is>
       </c>
     </row>
@@ -569,19 +569,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>levi, zach</t>
+          <t>worker 13, worker 14</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>meili, zach</t>
+          <t>worker 8, worker 15</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>makayla, brooklyn</t>
+          <t>worker 5, worker 11</t>
         </is>
       </c>
     </row>
@@ -593,27 +593,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>chloe, kacy, brooklyn, zach, tyler</t>
+          <t>worker 4, worker 7, worker 11, worker 14, worker 16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>andrew, brandon, kacy, levi, meili</t>
+          <t>worker 2, worker 3, worker 7, worker 8, worker 11</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>chloe, kacy, brooklyn, zach, troy</t>
+          <t>worker 3, worker 4, worker 7, worker 14, worker 15</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>andrew, eleanor, jess, kacy, brooklyn</t>
+          <t>worker 2, worker 3, worker 8, worker 11, worker 14</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>brandon, jess, makayla, thomas, brooklyn</t>
+          <t>worker 1, worker 3, worker 4, worker 6, worker 9</t>
         </is>
       </c>
     </row>
@@ -625,27 +625,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>amulek, brandon, kacy, brooklyn, tyler</t>
+          <t>worker 1, worker 7, worker 10, worker 11, worker 16</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>amulek, kacy, thomas, brooklyn, meili</t>
+          <t>worker 1, worker 6, worker 7, worker 11, worker 13</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>amulek, brandon, chloe, kacy, brooklyn</t>
+          <t>worker 1, worker 4, worker 7, worker 10, worker 11</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>amulek, brandon, jess, brooklyn, zach</t>
+          <t>worker 1, worker 6, worker 10, worker 11, worker 14</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>amulek, brandon, eleanor, makayla, tyler</t>
+          <t>worker 1, worker 5, worker 6, worker 9, worker 10</t>
         </is>
       </c>
     </row>
@@ -657,27 +657,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>amulek, chloe, kacy, maria</t>
+          <t>worker 3, worker 4, worker 11, worker 16</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>amulek, brandon, eleanor, brooklyn</t>
+          <t>worker 4, worker 9, worker 12, worker 13</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>amulek, brandon, chloe, thomas</t>
+          <t>worker 1, worker 3, worker 7, worker 12</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>brandon, jess, makayla, zach</t>
+          <t>worker 1, worker 4, worker 9, worker 11</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>makayla, brooklyn, maria, tyler</t>
+          <t>worker 1, worker 10, worker 11, worker 12</t>
         </is>
       </c>
     </row>
@@ -689,27 +689,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>amulek, andrew, levi, maria</t>
+          <t>worker 2, worker 4, worker 7, worker 12</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>chloe, levi, makayla, troy</t>
+          <t>worker 5, worker 8, worker 9, worker 11</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>amulek, andrew, levi, maria</t>
+          <t>worker 1, worker 2, worker 3, worker 8</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>chloe, brooklyn, maria, zach</t>
+          <t>worker 4, worker 9, worker 11, worker 14</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>amulek, andrew, chloe, levi</t>
+          <t>worker 1, worker 2, worker 4, worker 8</t>
         </is>
       </c>
     </row>
@@ -721,27 +721,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>amulek, andrew, makayla</t>
+          <t>worker 2, worker 4, worker 14</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>levi, makayla, brooklyn</t>
+          <t>worker 3, worker 11, worker 14</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>andrew, chloe, zach</t>
+          <t>worker 2, worker 9, worker 11</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>makayla, brooklyn, zach</t>
+          <t>worker 3, worker 8, worker 14</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>andrew, brandon, brooklyn</t>
+          <t>worker 1, worker 2, worker 8</t>
         </is>
       </c>
     </row>

</xml_diff>